<commit_message>
[Silverfox] FX 발주 / 플랫폼 추가
</commit_message>
<xml_diff>
--- a/DesignDocs/Design/발주 문서/FX발주.xlsx
+++ b/DesignDocs/Design/발주 문서/FX발주.xlsx
@@ -1,34 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\Design\발주 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA3CAB2-DE0F-4C47-AE89-D473EFEBE554}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" firstSheet="4" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" firstSheet="3" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2003" sheetId="1" r:id="rId1"/>
-    <sheet name="2004" sheetId="2" r:id="rId2"/>
-    <sheet name="2005" sheetId="3" r:id="rId3"/>
-    <sheet name="2006" sheetId="4" r:id="rId4"/>
-    <sheet name="2007" sheetId="5" r:id="rId5"/>
-    <sheet name="2008" sheetId="6" r:id="rId6"/>
-    <sheet name="2009, 2010, 2011" sheetId="7" r:id="rId7"/>
-    <sheet name="2013" sheetId="8" r:id="rId8"/>
-    <sheet name="2014" sheetId="9" r:id="rId9"/>
-    <sheet name="2015" sheetId="10" r:id="rId10"/>
-    <sheet name="2016" sheetId="11" r:id="rId11"/>
-    <sheet name="2017" sheetId="12" r:id="rId12"/>
-    <sheet name="2018" sheetId="13" r:id="rId13"/>
-    <sheet name="2019" sheetId="15" r:id="rId14"/>
-    <sheet name="2020" sheetId="16" r:id="rId15"/>
-    <sheet name="2021" sheetId="17" r:id="rId16"/>
-    <sheet name="2022" sheetId="18" r:id="rId17"/>
+    <sheet name="개요" sheetId="19" r:id="rId1"/>
+    <sheet name="2003" sheetId="20" r:id="rId2"/>
+    <sheet name="2004" sheetId="21" r:id="rId3"/>
+    <sheet name="2005" sheetId="22" r:id="rId4"/>
+    <sheet name="2006" sheetId="23" r:id="rId5"/>
+    <sheet name="2007" sheetId="24" r:id="rId6"/>
+    <sheet name="2008" sheetId="25" r:id="rId7"/>
+    <sheet name="2009~2011" sheetId="26" r:id="rId8"/>
+    <sheet name="2013" sheetId="27" r:id="rId9"/>
+    <sheet name="2014" sheetId="28" r:id="rId10"/>
+    <sheet name="2015" sheetId="29" r:id="rId11"/>
+    <sheet name="2016" sheetId="30" r:id="rId12"/>
+    <sheet name="2017" sheetId="31" r:id="rId13"/>
+    <sheet name="2018" sheetId="32" r:id="rId14"/>
+    <sheet name="2019" sheetId="33" r:id="rId15"/>
+    <sheet name="2020" sheetId="34" r:id="rId16"/>
+    <sheet name="2021" sheetId="35" r:id="rId17"/>
+    <sheet name="2022" sheetId="18" r:id="rId18"/>
+    <sheet name="2021 (2)" sheetId="36" r:id="rId19"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="56">
   <si>
     <t>OnStart</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,126 +61,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2000_OnHit0 노래색 바리에이션</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>melee</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2002_OnHit0 녹색 바리에이션</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>melee</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>노란색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>눈에서 안광번쩍 키랏</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bounce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>꽃에 따른 색상 바리에이션</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>약한 데미지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>melee</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>빛살번짐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>무지개 배리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>번개 휘감음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>번개 퍼짐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>소서리스 체인라이트닝</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bouce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고철로 모아 만든 둥그런 폭탄</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>맞은방향으로 고철이 퍼져나간다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>냉기가 휘어감음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>냉기 폭발</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>냉기 미사일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>낭아풍풍권</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>늑대 2번 할퀴기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>호랑이 1번 할퀴기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>휘감은 총알</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>강한타격</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>스팀압력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -187,13 +74,210 @@
   </si>
   <si>
     <t>증기탄화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enhancer Num.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnStart는 스킬을 사용할 때 시작되는 Fx이다.
+Ex) 오오라, 불꽃 휘감기 등</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnHit은 타격시 발생하는 FX이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Projectile은 투사체이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enhancer cid Num.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가로로 진공파와 같은 형태의 참격 FX가 발생한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>밀리 공격의 부분에 소닉붐 같이 3~4 Frame 정도 회전하는 FX가 발생한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Melee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000_Onhit0의 노란색 베리에이션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2002_Onhit0의 녹색 베리에이션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC의 몸 주변에 강한 기의 폭발과 같은 힘이 한번 방출된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2004와 동일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1~2 Frame의 긴 총구 화염</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>붉은색의 짧은 탄도 궤적
+탄도 궤적은 지속적으로 연결된 레이저포인트와 같은 역할이 아니라 짧은 궤적이 이동하는 투사체처럼 보인다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노랑/흰색의 타격 섬광</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2002_OnHit0의
+꽃색상 베리에이션 4종</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2008_Projectile0 / 2008_Projectile1 / 2008_Projectile2
+2008_Projectile3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>툭 던진 물건에 맞는 것 같은 약한 타격 FX로 크기가 크지 않게 빠르게 사라진다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Projectile은 투사체간 스왑을 위해 2009~2010을 공유하여 사용한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>투사체가 속도를 내는것 같이 공기를 가르는듯한 화살촉 모양을 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Projectile이 피격되면 주변으로 흰색 타격이 흩어져 사라진다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검은색 액체가 온몸을 휘감는듯 일렁거린다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검은 액체가 (상대적으로) 불규칙하게 사방으로 퍼진다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2009 ~ 2011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bounce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2003_Projectile0의 무지개 빛 베리에이션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몸 주변을 프리즘과 같은 무지개 빛이 살며시 감돈다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가둬진듯한 빛이 섬광탄처럼 살짝 번쩍 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Melee/Range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위의 레퍼런스와 비슷한 색상의 전기 자기장이 몸을 휘감는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강렬한 스파크가 3~4Frame 내에 번쩍 하며 대상을 통과한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일직선의 (상대적으로) 불규칙한 형태의 전기 줄기가 방출된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고철 뭉치가 발사되는 투사체의 역할을 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발사된 고철이 흩어지며 사라진다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>냉기가 PC의 몸을 살짝 휘감으며 반짝인다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>얼음 파편이 튄다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고드름이 반짝 거리며 투사체의 형태로 날아간다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC의 등 뒤로 늑대의 환영이 일렁거리며 올라온다.
+낭아풍풍권!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맹수가 할퀴는듯한 FX가 4 Frame 이내에 두번 촥촥 긁힌다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맹수가 할퀴는듯한 FX가 4 Frame 이내에 한번 촥 긁힌다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC의 등 뒤로 호랑이의 환영이 일렁거리며 올라온다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>투사체 자체는 2001_Projectile0의 베리에이션 형태로 사용하며 탄환 주위로 연기가 4Frame 이내로 휘감는게 반복된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피격되면 레퍼런스와 같이 3~4 Frame 이내에 연기 색상과 같은 후폭풍이 발생한다. (통배권?)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스팀에서 불꽃이 아닌 스팀이 강하게 뿜어져 나온다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스팀의 압력이 폭발하는듯한 수증기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탄환 자체의 묘사는 제한하고 스팀의 압력의 발사같은 느낌의 투사체</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -219,11 +303,39 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -233,11 +345,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -259,20 +383,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>512617</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>387927</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6079174</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>3505199</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3677974</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2189205</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D6815E7-4C60-4CBA-B98D-A2405548BCC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -291,8 +421,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1177635" y="4419600"/>
-          <a:ext cx="5566557" cy="3117272"/>
+          <a:off x="4438651" y="838200"/>
+          <a:ext cx="3535098" cy="1979655"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -303,26 +433,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3246782</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1490870</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6473687</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>3743739</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1743566</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1045793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3792844</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2476500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="도넛 2"/>
+        <xdr:cNvPr id="3" name="도넛 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED67169E-5329-486B-80C0-E9304608E79E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3916017" y="5519531"/>
-          <a:ext cx="3226905" cy="2252869"/>
+          <a:off x="6039341" y="1674443"/>
+          <a:ext cx="2049278" cy="1430707"/>
         </a:xfrm>
         <a:prstGeom prst="donut">
           <a:avLst>
@@ -366,20 +502,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>589721</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>284921</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6156278</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3402193</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>86630</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>211319</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3621728</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2190974</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDECC218-5498-4DD9-8DA4-308882741F39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -398,8 +540,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1258956" y="8123582"/>
-          <a:ext cx="5566557" cy="3117272"/>
+          <a:off x="8240030" y="839969"/>
+          <a:ext cx="3535098" cy="1979655"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -410,26 +552,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1223416</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>433708</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>4450321</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>2686577</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>720325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>360106</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2769603</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1790813</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="도넛 4"/>
+        <xdr:cNvPr id="5" name="도넛 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{913C7166-4700-44FF-B15F-35906539FF4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1892651" y="8272369"/>
-          <a:ext cx="3226905" cy="2252869"/>
+          <a:off x="8873725" y="988756"/>
+          <a:ext cx="2049278" cy="1430707"/>
         </a:xfrm>
         <a:prstGeom prst="donut">
           <a:avLst>
@@ -479,19 +627,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>917665</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>576942</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>5693228</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3246990</xdr:rowOff>
+      <xdr:colOff>3820117</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2162175</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="그림 5"/>
+        <xdr:cNvPr id="6" name="그림 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3359651-5DC3-4D7E-BFF9-8C8F25450AB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -510,8 +664,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1592579" y="794656"/>
-          <a:ext cx="4775563" cy="2670048"/>
+          <a:off x="476250" y="676275"/>
+          <a:ext cx="3782017" cy="2114550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -522,20 +676,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1810460</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>968829</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6422774</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2710542</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>64120</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>87088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3743160</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1476376</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="그림 6"/>
+        <xdr:cNvPr id="7" name="그림 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43C65FF8-A016-4C3B-A3A0-6B002E438336}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -554,8 +714,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2485374" y="4996543"/>
-          <a:ext cx="4612314" cy="1741713"/>
+          <a:off x="4359895" y="715738"/>
+          <a:ext cx="3679040" cy="1389288"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -566,20 +726,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1828800</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>315686</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>493814</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3432958</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>101511</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>91169</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3704715</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2105025</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="그림 7"/>
+        <xdr:cNvPr id="8" name="그림 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8515D710-153E-4D59-BF2E-A6F29AAF590C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -598,8 +764,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2503714" y="8153400"/>
-          <a:ext cx="5566557" cy="3117272"/>
+          <a:off x="8254911" y="719819"/>
+          <a:ext cx="3603204" cy="2013856"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -610,26 +776,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>4562965</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>1418629</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>213413</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3671498</xdr:rowOff>
+      <xdr:colOff>1911750</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>994087</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3524770</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2114550</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="도넛 8"/>
+        <xdr:cNvPr id="9" name="도넛 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A43E4D01-25BA-43EA-A981-661A9850347D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5237879" y="9256343"/>
-          <a:ext cx="3226905" cy="2252869"/>
+          <a:off x="10065150" y="1622737"/>
+          <a:ext cx="1613020" cy="1120463"/>
         </a:xfrm>
         <a:prstGeom prst="donut">
           <a:avLst>
@@ -679,19 +851,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2895600</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>272143</xdr:rowOff>
+      <xdr:colOff>93889</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>6515100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>2986768</xdr:rowOff>
+      <xdr:colOff>3713389</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2781300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPr id="6" name="그림 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E8DB6AD-4783-4C94-990E-5F9391F9522B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -710,7 +888,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3570514" y="489857"/>
+          <a:off x="532039" y="695325"/>
           <a:ext cx="3619500" cy="2714625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -722,20 +900,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1458686</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>533400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6792686</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>3533775</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>80283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3741360</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2152651</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPr id="7" name="그림 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9B17375-E831-48F3-8840-F8E812CC313D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -754,8 +938,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2133600" y="4561114"/>
-          <a:ext cx="5334000" cy="3000375"/>
+          <a:off x="4352925" y="708933"/>
+          <a:ext cx="3684210" cy="2072368"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -766,20 +950,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2100943</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>849086</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>5987143</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>2868386</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>80282</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>148318</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3714750</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2036816</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="그림 5"/>
+        <xdr:cNvPr id="8" name="그림 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C8E1480-B91E-4AD8-A2C1-BDEBB9421531}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -798,8 +988,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2775857" y="8686800"/>
-          <a:ext cx="3886200" cy="2019300"/>
+          <a:off x="8233682" y="776968"/>
+          <a:ext cx="3634468" cy="1888498"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -815,20 +1005,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2797629</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>511628</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6128658</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3058884</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3445329</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2642506</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1AF530D-D86D-4399-9281-EFF26AD5EC5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -847,7 +1043,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3472543" y="8349342"/>
+          <a:off x="8267700" y="723900"/>
           <a:ext cx="3331029" cy="2547256"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -865,19 +1061,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2645229</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>402771</xdr:rowOff>
+      <xdr:colOff>83004</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>6248401</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>2992551</xdr:rowOff>
+      <xdr:colOff>3686176</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2694555</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22A8D818-EBA9-42B8-880F-A95CC82A079D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -896,7 +1098,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3320143" y="620485"/>
+          <a:off x="521154" y="733425"/>
           <a:ext cx="3603172" cy="2589780"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -908,20 +1110,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2383972</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>370116</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6594022</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>87848</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>69397</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>110220</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3676650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3132850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6117B15-5792-4B24-A89C-DEED50E6883D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -940,8 +1148,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3058886" y="8207830"/>
-          <a:ext cx="4210050" cy="3527732"/>
+          <a:off x="8222797" y="738870"/>
+          <a:ext cx="3607253" cy="3022630"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -952,20 +1160,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2286000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3733801</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6496050</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>3451533</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>73480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3676650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3106372</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="그림 5"/>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB3A2399-3B7F-406D-A0BC-CC2804FBB860}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -984,8 +1198,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2960914" y="3951515"/>
-          <a:ext cx="4210050" cy="3527732"/>
+          <a:off x="4352925" y="702130"/>
+          <a:ext cx="3619500" cy="3032892"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -996,26 +1210,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>4386943</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1164772</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>5540829</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2166258</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2015218</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1266826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3007247</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2032844</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="도넛 7"/>
+        <xdr:cNvPr id="6" name="도넛 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{579DB426-D5AC-4013-9C30-06968ADD053E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5061857" y="5192486"/>
-          <a:ext cx="1153886" cy="1001486"/>
+          <a:off x="6310993" y="1895476"/>
+          <a:ext cx="992029" cy="766018"/>
         </a:xfrm>
         <a:prstGeom prst="donut">
           <a:avLst>
@@ -1059,26 +1279,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>5040086</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>2220686</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6193972</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3222172</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2477861</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1684565</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3466533</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2478009</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="도넛 8"/>
+        <xdr:cNvPr id="7" name="도넛 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76F2E0B4-F49F-4754-BC91-7CC105E43316}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5715000" y="10058400"/>
-          <a:ext cx="1153886" cy="1001486"/>
+          <a:off x="10631261" y="2313215"/>
+          <a:ext cx="988672" cy="793444"/>
         </a:xfrm>
         <a:prstGeom prst="donut">
           <a:avLst>
@@ -1128,19 +1354,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3864430</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>206829</xdr:rowOff>
+      <xdr:colOff>1536248</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>6085116</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3439565</xdr:rowOff>
+      <xdr:colOff>3756934</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3261311</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="그림 6"/>
+        <xdr:cNvPr id="7" name="그림 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01B8AEBD-676F-4123-9460-5BE584C59E9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1159,7 +1391,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4539344" y="424543"/>
+          <a:off x="1974398" y="657225"/>
           <a:ext cx="2220686" cy="3232736"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1171,20 +1403,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1785257</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>576942</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6489441</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>3211285</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>55789</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3704936</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2114551</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="그림 7"/>
+        <xdr:cNvPr id="8" name="그림 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDEAE459-0828-4E19-9AFA-C04488E94956}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1203,8 +1441,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2460171" y="4604656"/>
-          <a:ext cx="4704184" cy="2634343"/>
+          <a:off x="4324350" y="684439"/>
+          <a:ext cx="3676361" cy="2058762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1221,19 +1459,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1492477</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>348342</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>6430735</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3265713</xdr:rowOff>
+      <xdr:colOff>3790950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2307132</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9887CF47-6F16-4E67-BB1E-0283AE255520}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1252,8 +1496,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2167391" y="566056"/>
-          <a:ext cx="4938258" cy="2917371"/>
+          <a:off x="533400" y="752476"/>
+          <a:ext cx="3695700" cy="2183306"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1264,20 +1508,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1687286</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>424542</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6644174</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>3200399</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>51934</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3725863</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2190751</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFF4A4AA-9067-4A40-BCE4-3702E44A5B02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1296,8 +1546,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2362200" y="4452256"/>
-          <a:ext cx="4956888" cy="2775857"/>
+          <a:off x="4347709" y="762001"/>
+          <a:ext cx="3673929" cy="2057400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1313,20 +1563,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2680147</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>685800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6753225</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3083378</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>102955</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>138793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3648075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2225594</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A96C77C2-9A2E-4581-8933-659263A5EFD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1345,8 +1601,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3355061" y="8523514"/>
-          <a:ext cx="4073078" cy="2397578"/>
+          <a:off x="8256355" y="767443"/>
+          <a:ext cx="3545120" cy="2086801"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1357,20 +1613,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1186542</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1099457</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6687119</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2764972</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3790951</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1242844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="그림 5"/>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38B51A9F-72FE-4685-A3D0-EE8B314C42AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1388,8 +1650,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1861456" y="5127171"/>
-          <a:ext cx="5500577" cy="1665515"/>
+          <a:off x="4391026" y="752476"/>
+          <a:ext cx="3695700" cy="1119018"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1418,7 +1680,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1461,7 +1729,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1504,7 +1778,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1536,24 +1816,183 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>25853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2143125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1936560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F805907-0D4A-4923-A5E0-0DCF5B3A3EA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="32864" t="70210" r="51811"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4362450" y="654503"/>
+          <a:ext cx="2076450" cy="1910707"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>122463</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>58510</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2452006</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2363006</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27F9119B-1E72-4181-97AE-B8A4FDE26381}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="65912" t="33545" r="16917" b="30571"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8275863" y="687160"/>
+          <a:ext cx="2329543" cy="2304496"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>59872</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3705226</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2243369</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{810764A5-5F21-483F-9CA7-33EAFF4B258B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="498022" y="704850"/>
+          <a:ext cx="3645354" cy="2167169"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2852058</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1280886</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6302830</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2431143</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>590550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3307897</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1518557</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="그림 7"/>
+        <xdr:cNvPr id="6" name="그림 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCCD57AA-2616-4657-AFEE-35303855E2A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1572,8 +2011,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3526972" y="5308600"/>
-          <a:ext cx="3450772" cy="1150257"/>
+          <a:off x="4819650" y="1219200"/>
+          <a:ext cx="2784022" cy="928007"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1607,20 +2046,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2754087</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1132114</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>621146</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2645228</xdr:rowOff>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3710881</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1274988</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AA6C306-0F0C-420D-9642-2CCA37FAC655}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1639,8 +2084,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3429001" y="5159828"/>
-          <a:ext cx="4768602" cy="1513114"/>
+          <a:off x="4400550" y="761999"/>
+          <a:ext cx="3606106" cy="1141639"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1687,19 +2132,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2547257</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>337457</xdr:rowOff>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>6727372</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3217092</xdr:rowOff>
+      <xdr:colOff>3711063</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2495551</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDE96F5F-0685-4477-85B6-25B0E09D9CB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1718,8 +2169,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3222171" y="555171"/>
-          <a:ext cx="4180115" cy="2879635"/>
+          <a:off x="609600" y="685801"/>
+          <a:ext cx="3539613" cy="2438400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1735,20 +2186,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>631372</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>587828</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>5802086</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>3396060</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>144236</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3757084</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2076450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03320D19-54ED-4050-BA77-BC02B01A8B3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1767,8 +2224,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1306286" y="4615542"/>
-          <a:ext cx="5170714" cy="2808232"/>
+          <a:off x="4440011" y="742950"/>
+          <a:ext cx="3612848" cy="1962150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1779,20 +2236,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>620486</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>489857</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>5791200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3298089</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>34449</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3827688</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2114550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A563382-CB6B-4DBD-9AD9-4AB401DECDB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1811,8 +2274,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1295400" y="8327571"/>
-          <a:ext cx="5170714" cy="2808232"/>
+          <a:off x="8187849" y="683079"/>
+          <a:ext cx="3793239" cy="2060121"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1823,26 +2286,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3701144</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1284514</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>5018316</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2558143</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2271033</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>649062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3180575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1478848</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="도넛 4"/>
+        <xdr:cNvPr id="5" name="도넛 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8326549-2BF6-4B48-BE67-F5D85BA15411}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4376058" y="5312228"/>
-          <a:ext cx="1317172" cy="1273629"/>
+          <a:off x="6566808" y="1277712"/>
+          <a:ext cx="909542" cy="829786"/>
         </a:xfrm>
         <a:prstGeom prst="donut">
           <a:avLst>
@@ -1886,26 +2355,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1872344</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>729343</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3984172</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>2100943</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1315786</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>265340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2544536</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1271547</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="도넛 5"/>
+        <xdr:cNvPr id="6" name="도넛 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3DB624A-39C2-475B-9DA1-EC76EF596449}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2547258" y="8567057"/>
-          <a:ext cx="2111828" cy="1371600"/>
+          <a:off x="9469186" y="893990"/>
+          <a:ext cx="1228750" cy="1006207"/>
         </a:xfrm>
         <a:prstGeom prst="donut">
           <a:avLst>
@@ -1947,6 +2422,125 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3821814</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2212521</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="그림 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDF62B9E-0D59-48D6-9E46-E3C6E9834D85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="466725" y="781050"/>
+          <a:ext cx="3793239" cy="2060121"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>376462</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>182336</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1605212</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1188543</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="도넛 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2BB314D-15B9-4B08-B7A2-E09C821BF5FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="814612" y="810986"/>
+          <a:ext cx="1228750" cy="1006207"/>
+        </a:xfrm>
+        <a:prstGeom prst="donut">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 3873"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1954,20 +2548,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1981200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1045028</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6749802</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2558142</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>190774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3630760</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1276350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="그림 5"/>
+        <xdr:cNvPr id="8" name="그림 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97F7CA1E-7831-4474-B9C1-A8684BD1FDB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1986,8 +2586,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2656114" y="1262742"/>
-          <a:ext cx="4768602" cy="1513114"/>
+          <a:off x="4505324" y="819424"/>
+          <a:ext cx="3421211" cy="1085576"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2033,20 +2633,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3287486</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1262744</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6132287</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2862944</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3044826</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1752600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1038975D-54A4-4A33-BDE9-C5FB42E9A0B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2065,7 +2671,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3962400" y="5290458"/>
+          <a:off x="4495800" y="781050"/>
           <a:ext cx="2844801" cy="1600200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2082,20 +2688,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2939142</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>3744687</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6281058</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3704057</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>92526</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3434442</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>109049</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9ED4E88-9E95-4A1F-936F-A9F223BA43F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2114,7 +2726,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3614056" y="7772401"/>
+          <a:off x="8245926" y="359229"/>
           <a:ext cx="3341916" cy="3769370"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2126,20 +2738,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2122716</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1251858</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6253466</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2460172</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3752850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1153302</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF76CC34-C703-46AF-B828-EC0445BCACC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2157,8 +2775,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2797630" y="5279572"/>
-          <a:ext cx="4130750" cy="1208314"/>
+          <a:off x="4333875" y="695325"/>
+          <a:ext cx="3714750" cy="1086627"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2174,20 +2792,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>736352</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>413656</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6476999</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>3638549</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>63955</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>97973</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3653675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2114551</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7EF4403-3DCF-454E-B849-001E55643EC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2206,8 +2830,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1411266" y="4441370"/>
-          <a:ext cx="5740647" cy="3224893"/>
+          <a:off x="4359730" y="726623"/>
+          <a:ext cx="3589720" cy="2016578"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2219,19 +2843,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>529523</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>239484</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>6270170</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3464377</xdr:rowOff>
+      <xdr:colOff>3514725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2032887</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD8AC586-5530-491A-983C-8AB05F0BE204}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2250,8 +2880,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1204437" y="457198"/>
-          <a:ext cx="5740647" cy="3224893"/>
+          <a:off x="571500" y="762000"/>
+          <a:ext cx="3381375" cy="1899537"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2263,25 +2893,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2514601</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1110344</xdr:rowOff>
+      <xdr:colOff>1327854</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>908960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>5741506</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3363213</xdr:rowOff>
+      <xdr:colOff>3228576</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1953645</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="도넛 5"/>
+        <xdr:cNvPr id="6" name="도넛 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{188FCF1C-494B-41F3-8F12-E20056CA5DB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3189515" y="1328058"/>
-          <a:ext cx="3226905" cy="2252869"/>
+          <a:off x="1766004" y="1537610"/>
+          <a:ext cx="1900722" cy="1044685"/>
         </a:xfrm>
         <a:prstGeom prst="donut">
           <a:avLst>
@@ -2325,26 +2961,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>555172</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1404258</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3782077</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>3657127</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1088575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1683297</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2066925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="도넛 6"/>
+        <xdr:cNvPr id="7" name="도넛 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E9E05DC-7E4D-4FD7-BFAD-38DC5640E141}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1230086" y="5431972"/>
-          <a:ext cx="3226905" cy="2252869"/>
+          <a:off x="4667250" y="1717225"/>
+          <a:ext cx="1311822" cy="978350"/>
         </a:xfrm>
         <a:prstGeom prst="donut">
           <a:avLst>
@@ -2651,40 +3293,573 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76E5F92-AC3C-4D2E-A2CF-A1F8888B9C31}">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB17FA8-D7D3-40E1-8D7D-1AE194B95091}">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2014</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D96764-1E95-49EC-A405-E715A5BBEE11}">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2015</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4248221C-A483-4C8D-8B4E-0F11F38AB1E4}">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2016</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497811AC-5732-4A65-A6E8-CED6CE866876}">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B2:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2017</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2859E6-BBFE-4043-A839-0DBF3247075F}">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2018</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3158442-BDDD-441C-8B26-A691DC88D033}">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2019</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30203166-A2BC-433E-9B0A-67CA5F2CD486}">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2019</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE59680-81DA-40DA-B616-D4E5F497A551}">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2019</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
+    <col min="2" max="2" width="90.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2694,778 +3869,530 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8B4025-6053-4436-A07F-AEED9CEF9B6B}">
+  <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2019</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>18</v>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2CB762-B550-4919-8CC4-763DD49CCD52}">
+  <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2003</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D1ED59-8AD5-4123-BA7A-DCA3CCBAC6E3}">
+  <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2004</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB724494-E393-44AD-97A2-43F672F69B12}">
+  <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2005</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A832E39-4736-4636-94AE-2414158968E6}">
+  <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2006</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD7CEC4-F0C0-4FB3-A2DA-7975C7D638FD}">
+  <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2007</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26C303F-7799-466C-AD31-36B5A4D85A3C}">
+  <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2008</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29594F0-4D6B-46D8-A5CF-E9923FB1FDDB}">
+  <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F01E83-3494-4928-870B-26C9DC24AC0D}">
+  <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.59765625" customWidth="1"/>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2013</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Silverfox] FX 발주 문서 수정
</commit_message>
<xml_diff>
--- a/DesignDocs/Design/발주 문서/FX발주.xlsx
+++ b/DesignDocs/Design/발주 문서/FX발주.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\Design\발주 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA3CAB2-DE0F-4C47-AE89-D473EFEBE554}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067005DD-47E4-41B2-8150-606E65455385}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" firstSheet="3" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="개요" sheetId="19" r:id="rId1"/>
@@ -30,8 +30,7 @@
     <sheet name="2019" sheetId="33" r:id="rId15"/>
     <sheet name="2020" sheetId="34" r:id="rId16"/>
     <sheet name="2021" sheetId="35" r:id="rId17"/>
-    <sheet name="2022" sheetId="18" r:id="rId18"/>
-    <sheet name="2021 (2)" sheetId="36" r:id="rId19"/>
+    <sheet name="2022" sheetId="36" r:id="rId18"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="62">
   <si>
     <t>OnStart</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -54,26 +53,6 @@
   </si>
   <si>
     <t>Projectile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>설명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>melee</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스팀압력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>뭉개뭉개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>증기탄화</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -271,6 +250,50 @@
   </si>
   <si>
     <t>탄환 자체의 묘사는 제한하고 스팀의 압력의 발사같은 느낌의 투사체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64/96</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64/96</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32/32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32/32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32/16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08 * 08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 * 16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64*96</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32*16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16*16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8*8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -278,6 +301,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -345,11 +371,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -361,6 +386,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1664,159 +1695,6 @@
 </file>
 
 <file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2177143</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>522514</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>5758543</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>8045</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="32864" t="70210" r="51811"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2852057" y="4550228"/>
-          <a:ext cx="3581400" cy="3295531"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3842656</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>1012371</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6172199</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3316867</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="65912" t="33545" r="16917" b="30571"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4517570" y="8850085"/>
-          <a:ext cx="2329543" cy="2304496"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2503714</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>849086</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6348951</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3135086</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3178628" y="1066800"/>
-          <a:ext cx="3845237" cy="2286000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3307,36 +3185,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4"/>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3348,10 +3226,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB17FA8-D7D3-40E1-8D7D-1AE194B95091}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3361,40 +3239,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
         <v>2014</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="5"/>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3406,67 +3292,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D96764-1E95-49EC-A405-E715A5BBEE11}">
-  <dimension ref="B2:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.75" customWidth="1"/>
-    <col min="2" max="4" width="50.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2015</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4248221C-A483-4C8D-8B4E-0F11F38AB1E4}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -3479,41 +3305,120 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2015</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4248221C-A483-4C8D-8B4E-0F11F38AB1E4}">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
         <v>2016</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>38</v>
+      <c r="D2" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>41</v>
+      <c r="B5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3526,10 +3431,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497811AC-5732-4A65-A6E8-CED6CE866876}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B2:D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3539,39 +3444,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
         <v>2017</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>42</v>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -3584,67 +3497,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2859E6-BBFE-4043-A839-0DBF3247075F}">
-  <dimension ref="B2:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.75" customWidth="1"/>
-    <col min="2" max="4" width="50.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2018</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3158442-BDDD-441C-8B26-A691DC88D033}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -3657,40 +3510,119 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3158442-BDDD-441C-8B26-A691DC88D033}">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
         <v>2019</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="5"/>
+      <c r="B5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3702,10 +3634,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30203166-A2BC-433E-9B0A-67CA5F2CD486}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3715,40 +3647,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
         <v>2019</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="5"/>
+      <c r="B5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3760,7 +3700,144 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE59680-81DA-40DA-B616-D4E5F497A551}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8B4025-6053-4436-A07F-AEED9CEF9B6B}">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2CB762-B550-4919-8CC4-763DD49CCD52}">
+  <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -3773,213 +3850,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2019</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2003</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="90.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="300" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8B4025-6053-4436-A07F-AEED9CEF9B6B}">
-  <dimension ref="B2:D5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.75" customWidth="1"/>
-    <col min="2" max="4" width="50.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2019</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2CB762-B550-4919-8CC4-763DD49CCD52}">
-  <dimension ref="B2:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.75" customWidth="1"/>
-    <col min="2" max="4" width="50.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2003</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4004,40 +3915,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
         <v>2004</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4062,40 +3973,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2005</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4">
-        <v>2005</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4107,10 +4018,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A832E39-4736-4636-94AE-2414158968E6}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4120,40 +4031,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
         <v>2006</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="5"/>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4178,41 +4096,41 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
         <v>2007</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>22</v>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -4228,7 +4146,7 @@
   <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4238,39 +4156,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
         <v>2008</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>34</v>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>25</v>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -4286,7 +4204,7 @@
   <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4296,39 +4214,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>27</v>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -4354,39 +4272,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
         <v>2013</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>28</v>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Silverfox] FX 레퍼런스 추가
</commit_message>
<xml_diff>
--- a/DesignDocs/Design/발주 문서/FX발주.xlsx
+++ b/DesignDocs/Design/발주 문서/FX발주.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\Design\발주 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067005DD-47E4-41B2-8150-606E65455385}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2920B308-064D-4FF7-9E0E-6127CE17CF47}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="개요" sheetId="19" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="63">
   <si>
     <t>OnStart</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -294,6 +294,10 @@
   </si>
   <si>
     <t>8*8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64*96</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1029,6 +1033,138 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>94599</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2809875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2028410</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>5171569</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4A52552-0C6E-48BF-8BCC-1E2B0C494F57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="532749" y="3438525"/>
+          <a:ext cx="1933811" cy="2361694"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114315</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2162163</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1571458</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3371687</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFDF45C5-C61E-4A52-BEF7-54AEC86271B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="8391525" y="2667003"/>
+          <a:ext cx="1209524" cy="1457143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2219325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3200006</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3066944</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{185C042A-76C1-4C22-A37D-C3CC8DF7DEAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4343400" y="2847975"/>
+          <a:ext cx="3152381" cy="847619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1375,6 +1511,94 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3171825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3704765</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4809920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3B534CF-DFE8-48D0-AA39-C434903B341F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4324350" y="3800475"/>
+          <a:ext cx="3676190" cy="1638095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3209925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1438105</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4086115</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{294F97EB-6A02-44F2-A095-5E18AEAA56AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8229600" y="3838575"/>
+          <a:ext cx="1361905" cy="876190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3362,8 +3586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4248221C-A483-4C8D-8B4E-0F11F38AB1E4}">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3394,7 +3618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3433,7 +3657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497811AC-5732-4A65-A6E8-CED6CE866876}">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -3500,7 +3724,7 @@
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3531,7 +3755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3702,7 +3926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE59680-81DA-40DA-B616-D4E5F497A551}">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -4143,10 +4367,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26C303F-7799-466C-AD31-36B5A4D85A3C}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4189,6 +4413,11 @@
       </c>
       <c r="D5" s="4" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -4203,8 +4432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29594F0-4D6B-46D8-A5CF-E9923FB1FDDB}">
   <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[Silverfox] FX 추가 발주 2025까지 / NPC 수정
</commit_message>
<xml_diff>
--- a/DesignDocs/Design/발주 문서/FX발주.xlsx
+++ b/DesignDocs/Design/발주 문서/FX발주.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\Design\발주 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2920B308-064D-4FF7-9E0E-6127CE17CF47}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C364FCD-2638-4665-B77E-5ABB66A59262}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" firstSheet="15" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="개요" sheetId="19" r:id="rId1"/>
@@ -31,6 +31,9 @@
     <sheet name="2020" sheetId="34" r:id="rId16"/>
     <sheet name="2021" sheetId="35" r:id="rId17"/>
     <sheet name="2022" sheetId="36" r:id="rId18"/>
+    <sheet name="2023" sheetId="38" r:id="rId19"/>
+    <sheet name="2024" sheetId="40" r:id="rId20"/>
+    <sheet name="2025" sheetId="42" r:id="rId21"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="73">
   <si>
     <t>OnStart</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -298,6 +301,46 @@
   </si>
   <si>
     <t>64*96</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스팀에서 불꽃이 퐁- 하고 나온다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>투사체 자체가 느릿한 형태의 불꽃이 날아가는 형태이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16*8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>충돌시 화염이 대상을 순간적으로 휘감는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구형의 에너지 형태 투사체 주변으로 원자 같이 작은 투사체가 빙글빙글 돌고 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>충돌시 강한 에너지의 형태가 대상을 순간적으로 휘감으며 다른 색상(보색이었으면 좋겠음)과 4Frame 이내에서 두번 점멸한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공학적인 느낌의 에너지 투사체의 힘이 나오는 형태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>투박한 형태의 흙먼지가 총기에서 튀어 나오는 형태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>충돌시 흙먼지가 뒤로 날리는 느낌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>암석의 형태로 뭉쳐진 투사체가 빙글빙글 구르며 날아간다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2071,6 +2114,280 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2352390</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>600017</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B70C3E5-7CB1-419C-ABE6-42790D1D8C45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="514350" y="762000"/>
+          <a:ext cx="2276190" cy="466667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>172059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3647554</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>628581</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E3BFC79-4CCD-4365-9785-7BFC2F9E18E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8353425" y="800709"/>
+          <a:ext cx="3447529" cy="456522"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3800473</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>723900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="그림 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBAD2479-3D33-4C4F-BFB6-A342A80FCC45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4381500" y="733425"/>
+          <a:ext cx="3714748" cy="619125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3753884</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2114550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD191EA0-E20F-4134-BBB3-A3DCBE5511DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8220075" y="742950"/>
+          <a:ext cx="3687209" cy="2000250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>295274</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3057524</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1975947</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEF327E5-1780-4A6A-A40D-8F3E579D380E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4543424" y="923924"/>
+          <a:ext cx="2809875" cy="1680673"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3800475</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>813216</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="그림 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1110E521-FB77-4B90-8032-147A20DB1841}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="476250" y="714376"/>
+          <a:ext cx="3762375" cy="727490"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2137,6 +2454,187 @@
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3671474</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1152525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB834DCB-0061-4BD3-ABEE-8309A245F6EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="495300" y="704850"/>
+          <a:ext cx="3614324" cy="1076325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3358641</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1133474</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A3398B5-E81D-48E3-98B6-BB5F9785842D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4362449" y="704849"/>
+          <a:ext cx="3291967" cy="1057275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2749394</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>952499</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="그림 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72F104D4-7233-45C6-9D0F-0E1EBBF10231}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8172450" y="714374"/>
+          <a:ext cx="2730344" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1000125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3257151</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1990601</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9FB71DA-022D-45CE-A157-63788EC1463E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8220075" y="1628775"/>
+          <a:ext cx="3190476" cy="990476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -3926,7 +4424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE59680-81DA-40DA-B616-D4E5F497A551}">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -3993,7 +4491,7 @@
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4049,6 +4547,77 @@
       </c>
       <c r="D6" s="5" t="s">
         <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C02F4D-64EE-403A-9EF8-07751C379322}">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -4124,6 +4693,148 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAE6FC8-3DB0-47DC-AE47-A3E8AA72F4C7}">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2024</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F365A3-724E-477D-A806-CD15364FA0A2}">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2025</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D1ED59-8AD5-4123-BA7A-DCA3CCBAC6E3}">
   <dimension ref="B2:D5"/>

</xml_diff>

<commit_message>
[Silverfox] 블룸의 스킬 Fx 수정
</commit_message>
<xml_diff>
--- a/DesignDocs/Design/발주 문서/FX발주.xlsx
+++ b/DesignDocs/Design/발주 문서/FX발주.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\Design\발주 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC71E4AF-3186-4121-8F7D-44EB01B0AD96}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B2DCEE-55F1-441E-B3E0-DDE110C39DF7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" firstSheet="11" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" firstSheet="12" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="개요" sheetId="19" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="2024" sheetId="40" r:id="rId20"/>
     <sheet name="2025" sheetId="42" r:id="rId21"/>
     <sheet name="6143" sheetId="44" r:id="rId22"/>
+    <sheet name="6144" sheetId="45" r:id="rId23"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="77">
   <si>
     <t>OnStart</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -352,6 +353,14 @@
   <si>
     <t>충격파를 발사하는 끝 형태
 파동이 사방으로 퍼져 나가는 부분 (보라색)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64*128</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>녹색의 독가스 구름의 기둥</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2879,6 +2888,55 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>18570</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2209549</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{230666BC-AE64-46D7-88A0-0572A43E6073}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="476250" y="828675"/>
+          <a:ext cx="3838095" cy="2009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5081,8 +5139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB27663-7D38-4248-BBE4-66665FE19D06}">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5134,6 +5192,68 @@
       <c r="D6" s="5" t="s">
         <v>65</v>
       </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E12392-CCFC-4809-BC6D-EC136BB76E66}">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="2" max="4" width="50.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>6144</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>